<commit_message>
initial mapping of pns
</commit_message>
<xml_diff>
--- a/Templates/BluePrint.xlsx
+++ b/Templates/BluePrint.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="6" xr2:uid="{791BE3AC-23BD-49AA-B912-E6D81B31C45D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="7" xr2:uid="{791BE3AC-23BD-49AA-B912-E6D81B31C45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1714" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1858" uniqueCount="704">
   <si>
     <t>Id</t>
   </si>
@@ -2023,6 +2023,126 @@
   </si>
   <si>
     <t>TestingRemarks</t>
+  </si>
+  <si>
+    <t>ObsPartnerScreening</t>
+  </si>
+  <si>
+    <t>DTL_FBCUSTOMFIELD_PNSFORM</t>
+  </si>
+  <si>
+    <t>PnsScreeningDate</t>
+  </si>
+  <si>
+    <t>PnsAccepted</t>
+  </si>
+  <si>
+    <t>ScreenedIPV</t>
+  </si>
+  <si>
+    <t>IPVQuestionOne</t>
+  </si>
+  <si>
+    <t>IPVQuestionTwo</t>
+  </si>
+  <si>
+    <t>IPVQuestionThree</t>
+  </si>
+  <si>
+    <t>IPVOutcome</t>
+  </si>
+  <si>
+    <t>PNSOccupation</t>
+  </si>
+  <si>
+    <t>PNSRealtionship</t>
+  </si>
+  <si>
+    <t>PNSCurrentlyLivingWithClient</t>
+  </si>
+  <si>
+    <t>PNSKnowledgeHIVStatus</t>
+  </si>
+  <si>
+    <t>PNSApproach</t>
+  </si>
+  <si>
+    <t>ScreeningDate</t>
+  </si>
+  <si>
+    <t>Occupation</t>
+  </si>
+  <si>
+    <t>PhysicalAssult</t>
+  </si>
+  <si>
+    <t>Threatened</t>
+  </si>
+  <si>
+    <t>SexuallyUncomfortable</t>
+  </si>
+  <si>
+    <t>LivingWithClient</t>
+  </si>
+  <si>
+    <t>284cded0-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284ce132-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284ce4de-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284ce614-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284ce736-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284ce844-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284ce9c0-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284cec18-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284cefba-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284cf154-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284cf294-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>284cf3b6-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>a7d757d4-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>a7d75a2c-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>a7d75bee-0033-11e8-ba89-0ed5f89f718b</t>
+  </si>
+  <si>
+    <t>DTL_CUSTOMFORM_Contact Tracing and Outcomes_PNSTRACING</t>
+  </si>
+  <si>
+    <t>FT_Outcome</t>
+  </si>
+  <si>
+    <t>PNSMode</t>
+  </si>
+  <si>
+    <t>PNSConsent</t>
+  </si>
+  <si>
+    <t>2d5e1b6e-0038-11e8-ba89-0ed5f89f718b</t>
   </si>
 </sst>
 </file>
@@ -2177,14 +2297,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{87B17825-EC5C-4480-A566-6C034FCA05E3}" name="Table7" displayName="Table7" ref="A1:L40" totalsRowShown="0">
-  <autoFilter ref="A1:L40" xr:uid="{ACC6EB24-3A38-4B9D-B8B7-15B6862DD7D1}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="ObsFinalTestResult"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{87B17825-EC5C-4480-A566-6C034FCA05E3}" name="Table7" displayName="Table7" ref="A1:L52" totalsRowShown="0">
+  <autoFilter ref="A1:L52" xr:uid="{ACC6EB24-3A38-4B9D-B8B7-15B6862DD7D1}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{80C1A31B-4904-4DB0-94C4-0F3EB40A50F0}" name="Id"/>
     <tableColumn id="2" xr3:uid="{F54E4B7D-BE1A-4050-A714-DE4A799489AB}" name="Name"/>
@@ -2205,16 +2319,7 @@
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4E2AF602-AE1F-4015-8958-05DB5133E6C2}" name="Table8" displayName="Table8" ref="A1:J104" totalsRowShown="0">
-  <autoFilter ref="A1:J104" xr:uid="{C5189CF3-53F2-4CB5-A93F-FFF07CD5A6AE}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="ObsTestResult.Kit"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A2:J104">
-    <sortCondition ref="B1:B104"/>
-  </sortState>
+  <autoFilter ref="A1:J104" xr:uid="{C5189CF3-53F2-4CB5-A93F-FFF07CD5A6AE}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{9227F7C8-EE45-4CC9-B674-EE1A0F122C45}" name="Id"/>
     <tableColumn id="2" xr3:uid="{F792CF62-959A-4B86-98EF-A6FB625A5EED}" name="Ref"/>
@@ -5926,19 +6031,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42808880-C2B9-4DC7-82E0-A8AF856DED1E}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
@@ -5986,7 +6091,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>334</v>
       </c>
@@ -6018,7 +6123,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>340</v>
       </c>
@@ -6050,7 +6155,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>344</v>
       </c>
@@ -6082,7 +6187,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>347</v>
       </c>
@@ -6114,7 +6219,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>350</v>
       </c>
@@ -6146,7 +6251,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>353</v>
       </c>
@@ -6178,7 +6283,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>356</v>
       </c>
@@ -6210,7 +6315,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>359</v>
       </c>
@@ -6242,7 +6347,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>360</v>
       </c>
@@ -6280,7 +6385,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>364</v>
       </c>
@@ -6318,7 +6423,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>366</v>
       </c>
@@ -6356,7 +6461,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>369</v>
       </c>
@@ -6394,7 +6499,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>374</v>
       </c>
@@ -6432,7 +6537,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>377</v>
       </c>
@@ -6470,7 +6575,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>380</v>
       </c>
@@ -6508,7 +6613,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>383</v>
       </c>
@@ -6546,7 +6651,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>386</v>
       </c>
@@ -6584,7 +6689,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>388</v>
       </c>
@@ -6622,7 +6727,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>390</v>
       </c>
@@ -6660,7 +6765,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>392</v>
       </c>
@@ -6689,7 +6794,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>398</v>
       </c>
@@ -6718,7 +6823,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>401</v>
       </c>
@@ -6747,7 +6852,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>403</v>
       </c>
@@ -6776,7 +6881,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>406</v>
       </c>
@@ -6805,7 +6910,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>409</v>
       </c>
@@ -6834,7 +6939,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>412</v>
       </c>
@@ -6863,7 +6968,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>415</v>
       </c>
@@ -6892,7 +6997,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>418</v>
       </c>
@@ -6921,7 +7026,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>421</v>
       </c>
@@ -7110,7 +7215,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>438</v>
       </c>
@@ -7142,7 +7247,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>441</v>
       </c>
@@ -7174,7 +7279,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>390</v>
       </c>
@@ -7212,7 +7317,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>390</v>
       </c>
@@ -7282,10 +7387,619 @@
         <v>339</v>
       </c>
     </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>684</v>
+      </c>
+      <c r="B41" t="s">
+        <v>664</v>
+      </c>
+      <c r="C41" t="s">
+        <v>678</v>
+      </c>
+      <c r="D41" t="s">
+        <v>342</v>
+      </c>
+      <c r="E41" t="s">
+        <v>665</v>
+      </c>
+      <c r="F41" t="s">
+        <v>666</v>
+      </c>
+      <c r="G41" t="s">
+        <v>342</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="I41" t="s">
+        <v>260</v>
+      </c>
+      <c r="J41">
+        <v>76</v>
+      </c>
+      <c r="K41">
+        <v>1016</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>685</v>
+      </c>
+      <c r="B42" t="s">
+        <v>664</v>
+      </c>
+      <c r="C42" t="s">
+        <v>667</v>
+      </c>
+      <c r="D42" t="s">
+        <v>277</v>
+      </c>
+      <c r="E42" t="s">
+        <v>665</v>
+      </c>
+      <c r="F42" t="s">
+        <v>667</v>
+      </c>
+      <c r="G42" t="s">
+        <v>260</v>
+      </c>
+      <c r="H42">
+        <v>7</v>
+      </c>
+      <c r="I42" t="s">
+        <v>260</v>
+      </c>
+      <c r="J42">
+        <v>76</v>
+      </c>
+      <c r="K42">
+        <v>1016</v>
+      </c>
+      <c r="L42" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>686</v>
+      </c>
+      <c r="B43" t="s">
+        <v>664</v>
+      </c>
+      <c r="C43" t="s">
+        <v>36</v>
+      </c>
+      <c r="D43" t="s">
+        <v>277</v>
+      </c>
+      <c r="E43" t="s">
+        <v>665</v>
+      </c>
+      <c r="F43" t="s">
+        <v>668</v>
+      </c>
+      <c r="G43" t="s">
+        <v>260</v>
+      </c>
+      <c r="H43">
+        <v>7</v>
+      </c>
+      <c r="I43" t="s">
+        <v>260</v>
+      </c>
+      <c r="J43">
+        <v>76</v>
+      </c>
+      <c r="K43">
+        <v>1016</v>
+      </c>
+      <c r="L43" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>687</v>
+      </c>
+      <c r="B44" t="s">
+        <v>664</v>
+      </c>
+      <c r="C44" t="s">
+        <v>680</v>
+      </c>
+      <c r="D44" t="s">
+        <v>277</v>
+      </c>
+      <c r="E44" t="s">
+        <v>665</v>
+      </c>
+      <c r="F44" t="s">
+        <v>669</v>
+      </c>
+      <c r="G44" t="s">
+        <v>260</v>
+      </c>
+      <c r="H44">
+        <v>7</v>
+      </c>
+      <c r="I44" t="s">
+        <v>260</v>
+      </c>
+      <c r="J44">
+        <v>76</v>
+      </c>
+      <c r="K44">
+        <v>1016</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>688</v>
+      </c>
+      <c r="B45" t="s">
+        <v>664</v>
+      </c>
+      <c r="C45" t="s">
+        <v>681</v>
+      </c>
+      <c r="D45" t="s">
+        <v>277</v>
+      </c>
+      <c r="E45" t="s">
+        <v>665</v>
+      </c>
+      <c r="F45" t="s">
+        <v>670</v>
+      </c>
+      <c r="G45" t="s">
+        <v>260</v>
+      </c>
+      <c r="H45">
+        <v>7</v>
+      </c>
+      <c r="I45" t="s">
+        <v>260</v>
+      </c>
+      <c r="J45">
+        <v>76</v>
+      </c>
+      <c r="K45">
+        <v>1016</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>689</v>
+      </c>
+      <c r="B46" t="s">
+        <v>664</v>
+      </c>
+      <c r="C46" t="s">
+        <v>682</v>
+      </c>
+      <c r="D46" t="s">
+        <v>277</v>
+      </c>
+      <c r="E46" t="s">
+        <v>665</v>
+      </c>
+      <c r="F46" t="s">
+        <v>671</v>
+      </c>
+      <c r="G46" t="s">
+        <v>260</v>
+      </c>
+      <c r="H46">
+        <v>7</v>
+      </c>
+      <c r="I46" t="s">
+        <v>260</v>
+      </c>
+      <c r="J46">
+        <v>76</v>
+      </c>
+      <c r="K46">
+        <v>1016</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>690</v>
+      </c>
+      <c r="B47" t="s">
+        <v>664</v>
+      </c>
+      <c r="C47" t="s">
+        <v>672</v>
+      </c>
+      <c r="D47" t="s">
+        <v>277</v>
+      </c>
+      <c r="E47" t="s">
+        <v>665</v>
+      </c>
+      <c r="F47" t="s">
+        <v>672</v>
+      </c>
+      <c r="G47" t="s">
+        <v>260</v>
+      </c>
+      <c r="H47">
+        <v>7</v>
+      </c>
+      <c r="I47" t="s">
+        <v>260</v>
+      </c>
+      <c r="J47">
+        <v>76</v>
+      </c>
+      <c r="K47">
+        <v>1016</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>691</v>
+      </c>
+      <c r="B48" t="s">
+        <v>664</v>
+      </c>
+      <c r="C48" t="s">
+        <v>679</v>
+      </c>
+      <c r="D48" t="s">
+        <v>277</v>
+      </c>
+      <c r="E48" t="s">
+        <v>665</v>
+      </c>
+      <c r="F48" t="s">
+        <v>673</v>
+      </c>
+      <c r="G48" t="s">
+        <v>277</v>
+      </c>
+      <c r="H48">
+        <v>7</v>
+      </c>
+      <c r="I48" t="s">
+        <v>260</v>
+      </c>
+      <c r="J48">
+        <v>77</v>
+      </c>
+      <c r="K48">
+        <v>1016</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>692</v>
+      </c>
+      <c r="B49" t="s">
+        <v>664</v>
+      </c>
+      <c r="C49" t="s">
+        <v>674</v>
+      </c>
+      <c r="D49" t="s">
+        <v>277</v>
+      </c>
+      <c r="E49" t="s">
+        <v>665</v>
+      </c>
+      <c r="F49" t="s">
+        <v>674</v>
+      </c>
+      <c r="G49" t="s">
+        <v>260</v>
+      </c>
+      <c r="H49">
+        <v>7</v>
+      </c>
+      <c r="I49" t="s">
+        <v>260</v>
+      </c>
+      <c r="J49">
+        <v>77</v>
+      </c>
+      <c r="K49">
+        <v>1016</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>693</v>
+      </c>
+      <c r="B50" t="s">
+        <v>664</v>
+      </c>
+      <c r="C50" t="s">
+        <v>683</v>
+      </c>
+      <c r="D50" t="s">
+        <v>277</v>
+      </c>
+      <c r="E50" t="s">
+        <v>665</v>
+      </c>
+      <c r="F50" t="s">
+        <v>675</v>
+      </c>
+      <c r="G50" t="s">
+        <v>260</v>
+      </c>
+      <c r="H50">
+        <v>7</v>
+      </c>
+      <c r="I50" t="s">
+        <v>260</v>
+      </c>
+      <c r="J50">
+        <v>77</v>
+      </c>
+      <c r="K50">
+        <v>1016</v>
+      </c>
+      <c r="L50" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>694</v>
+      </c>
+      <c r="B51" t="s">
+        <v>664</v>
+      </c>
+      <c r="C51" t="s">
+        <v>635</v>
+      </c>
+      <c r="D51" t="s">
+        <v>277</v>
+      </c>
+      <c r="E51" t="s">
+        <v>665</v>
+      </c>
+      <c r="F51" t="s">
+        <v>676</v>
+      </c>
+      <c r="G51" t="s">
+        <v>260</v>
+      </c>
+      <c r="H51">
+        <v>7</v>
+      </c>
+      <c r="I51" t="s">
+        <v>260</v>
+      </c>
+      <c r="J51">
+        <v>77</v>
+      </c>
+      <c r="K51">
+        <v>1016</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>695</v>
+      </c>
+      <c r="B52" t="s">
+        <v>664</v>
+      </c>
+      <c r="C52" t="s">
+        <v>677</v>
+      </c>
+      <c r="D52" t="s">
+        <v>277</v>
+      </c>
+      <c r="E52" t="s">
+        <v>665</v>
+      </c>
+      <c r="F52" t="s">
+        <v>677</v>
+      </c>
+      <c r="G52" t="s">
+        <v>260</v>
+      </c>
+      <c r="H52">
+        <v>7</v>
+      </c>
+      <c r="I52" t="s">
+        <v>260</v>
+      </c>
+      <c r="J52">
+        <v>77</v>
+      </c>
+      <c r="K52">
+        <v>1016</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>696</v>
+      </c>
+      <c r="B53" t="s">
+        <v>361</v>
+      </c>
+      <c r="C53" t="s">
+        <v>331</v>
+      </c>
+      <c r="D53" t="s">
+        <v>277</v>
+      </c>
+      <c r="E53" t="s">
+        <v>699</v>
+      </c>
+      <c r="F53" t="s">
+        <v>701</v>
+      </c>
+      <c r="G53" t="s">
+        <v>277</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53" t="s">
+        <v>265</v>
+      </c>
+      <c r="J53">
+        <v>72</v>
+      </c>
+      <c r="K53">
+        <v>1013</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>697</v>
+      </c>
+      <c r="B54" t="s">
+        <v>361</v>
+      </c>
+      <c r="C54" t="s">
+        <v>342</v>
+      </c>
+      <c r="D54" t="s">
+        <v>342</v>
+      </c>
+      <c r="E54" t="s">
+        <v>699</v>
+      </c>
+      <c r="F54" t="s">
+        <v>365</v>
+      </c>
+      <c r="G54" t="s">
+        <v>342</v>
+      </c>
+      <c r="H54">
+        <v>2</v>
+      </c>
+      <c r="I54" t="s">
+        <v>265</v>
+      </c>
+      <c r="J54">
+        <v>72</v>
+      </c>
+      <c r="K54">
+        <v>1013</v>
+      </c>
+      <c r="L54" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>698</v>
+      </c>
+      <c r="B55" t="s">
+        <v>361</v>
+      </c>
+      <c r="C55" t="s">
+        <v>367</v>
+      </c>
+      <c r="D55" t="s">
+        <v>277</v>
+      </c>
+      <c r="E55" t="s">
+        <v>699</v>
+      </c>
+      <c r="F55" t="s">
+        <v>700</v>
+      </c>
+      <c r="G55" t="s">
+        <v>277</v>
+      </c>
+      <c r="H55">
+        <v>2</v>
+      </c>
+      <c r="I55" t="s">
+        <v>265</v>
+      </c>
+      <c r="J55">
+        <v>72</v>
+      </c>
+      <c r="K55">
+        <v>1013</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>703</v>
+      </c>
+      <c r="B56" t="s">
+        <v>361</v>
+      </c>
+      <c r="C56" t="s">
+        <v>267</v>
+      </c>
+      <c r="D56" t="s">
+        <v>277</v>
+      </c>
+      <c r="E56" t="s">
+        <v>699</v>
+      </c>
+      <c r="F56" t="s">
+        <v>702</v>
+      </c>
+      <c r="G56" t="s">
+        <v>277</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56" t="s">
+        <v>265</v>
+      </c>
+      <c r="J56">
+        <v>72</v>
+      </c>
+      <c r="K56">
+        <v>1013</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -7294,7 +8008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9EDC7D2-F164-4AF1-BE00-B6B43F85EA47}">
   <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
@@ -7344,7 +8058,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>500</v>
       </c>
@@ -7376,7 +8090,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>502</v>
       </c>
@@ -7408,7 +8122,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>592</v>
       </c>
@@ -7440,7 +8154,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>593</v>
       </c>
@@ -7472,7 +8186,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>554</v>
       </c>
@@ -7504,7 +8218,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>556</v>
       </c>
@@ -7536,7 +8250,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>558</v>
       </c>
@@ -7568,7 +8282,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>560</v>
       </c>
@@ -7600,7 +8314,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>562</v>
       </c>
@@ -7632,7 +8346,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>564</v>
       </c>
@@ -7664,7 +8378,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>566</v>
       </c>
@@ -7696,7 +8410,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>568</v>
       </c>
@@ -7728,7 +8442,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>570</v>
       </c>
@@ -7760,7 +8474,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>572</v>
       </c>
@@ -7792,7 +8506,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>574</v>
       </c>
@@ -7824,7 +8538,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>576</v>
       </c>
@@ -7856,7 +8570,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>578</v>
       </c>
@@ -7888,7 +8602,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>580</v>
       </c>
@@ -7920,7 +8634,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>582</v>
       </c>
@@ -7952,7 +8666,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>584</v>
       </c>
@@ -7984,7 +8698,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>586</v>
       </c>
@@ -8016,7 +8730,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>588</v>
       </c>
@@ -8048,7 +8762,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>590</v>
       </c>
@@ -8080,7 +8794,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>518</v>
       </c>
@@ -8112,7 +8826,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>521</v>
       </c>
@@ -8144,7 +8858,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>524</v>
       </c>
@@ -8176,7 +8890,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>527</v>
       </c>
@@ -8208,7 +8922,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>530</v>
       </c>
@@ -8240,7 +8954,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>533</v>
       </c>
@@ -8272,7 +8986,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>504</v>
       </c>
@@ -8304,7 +9018,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>505</v>
       </c>
@@ -8336,7 +9050,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>536</v>
       </c>
@@ -8368,7 +9082,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>539</v>
       </c>
@@ -8400,7 +9114,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>506</v>
       </c>
@@ -8432,7 +9146,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>508</v>
       </c>
@@ -8464,7 +9178,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>510</v>
       </c>
@@ -8496,7 +9210,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>512</v>
       </c>
@@ -8528,7 +9242,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>514</v>
       </c>
@@ -8560,7 +9274,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>516</v>
       </c>
@@ -8592,7 +9306,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>542</v>
       </c>
@@ -8624,7 +9338,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>545</v>
       </c>
@@ -8656,7 +9370,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>548</v>
       </c>
@@ -8688,7 +9402,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>551</v>
       </c>
@@ -8720,7 +9434,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>614</v>
       </c>
@@ -8752,7 +9466,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>619</v>
       </c>
@@ -8784,7 +9498,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>622</v>
       </c>
@@ -8816,7 +9530,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>624</v>
       </c>
@@ -8848,7 +9562,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>628</v>
       </c>
@@ -8880,7 +9594,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>638</v>
       </c>
@@ -8906,7 +9620,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>634</v>
       </c>
@@ -8938,7 +9652,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>636</v>
       </c>
@@ -8970,7 +9684,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>637</v>
       </c>
@@ -8996,7 +9710,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>452</v>
       </c>
@@ -9025,7 +9739,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>455</v>
       </c>
@@ -9054,7 +9768,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="56" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>459</v>
       </c>
@@ -9083,7 +9797,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>462</v>
       </c>
@@ -9112,7 +9826,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="58" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>464</v>
       </c>
@@ -9141,7 +9855,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="59" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>467</v>
       </c>
@@ -9170,7 +9884,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>470</v>
       </c>
@@ -9199,7 +9913,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>471</v>
       </c>
@@ -9228,7 +9942,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>610</v>
       </c>
@@ -9260,7 +9974,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>612</v>
       </c>
@@ -9292,7 +10006,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>613</v>
       </c>
@@ -9324,7 +10038,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>602</v>
       </c>
@@ -9356,7 +10070,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>604</v>
       </c>
@@ -9388,7 +10102,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>605</v>
       </c>
@@ -9420,7 +10134,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>594</v>
       </c>
@@ -9452,7 +10166,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>596</v>
       </c>
@@ -9484,7 +10198,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>597</v>
       </c>
@@ -9516,7 +10230,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>607</v>
       </c>
@@ -9548,7 +10262,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>609</v>
       </c>
@@ -9580,7 +10294,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>598</v>
       </c>
@@ -9612,7 +10326,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>600</v>
       </c>
@@ -9644,7 +10358,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>601</v>
       </c>
@@ -9868,7 +10582,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>490</v>
       </c>
@@ -9900,7 +10614,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>493</v>
       </c>
@@ -9932,7 +10646,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>494</v>
       </c>
@@ -9964,7 +10678,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>496</v>
       </c>
@@ -9996,7 +10710,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>497</v>
       </c>
@@ -10028,7 +10742,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>499</v>
       </c>
@@ -10060,7 +10774,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>477</v>
       </c>
@@ -10092,7 +10806,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>479</v>
       </c>
@@ -10124,7 +10838,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>473</v>
       </c>
@@ -10156,7 +10870,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>475</v>
       </c>
@@ -10188,7 +10902,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>476</v>
       </c>
@@ -10220,7 +10934,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>629</v>
       </c>
@@ -10252,7 +10966,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>633</v>
       </c>
@@ -10278,7 +10992,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>640</v>
       </c>
@@ -10310,7 +11024,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>643</v>
       </c>
@@ -10342,7 +11056,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>645</v>
       </c>
@@ -10374,7 +11088,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>648</v>
       </c>
@@ -10406,7 +11120,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>650</v>
       </c>
@@ -10438,7 +11152,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>652</v>
       </c>
@@ -10470,7 +11184,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>654</v>
       </c>
@@ -10502,7 +11216,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>657</v>
       </c>
@@ -10534,7 +11248,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>448</v>
       </c>
@@ -10563,7 +11277,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>450</v>
       </c>

</xml_diff>